<commit_message>
Fixed a bug within the python script to generate auto gen
</commit_message>
<xml_diff>
--- a/sheets/array_test_sheet.xlsx
+++ b/sheets/array_test_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ExcelPy\OdinAnalytics\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CC3D26-0B80-40E0-B311-88E9A147F331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0281AAF1-F172-4AF7-9424-A0BA92057CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{CC038B3D-5DA1-43AC-BE17-600265123F86}"/>
   </bookViews>
@@ -73,9 +73,6 @@
     <t>Submariner:15</t>
   </si>
   <si>
-    <t>Reverso:9</t>
-  </si>
-  <si>
     <t>Oyster Perpetual:15</t>
   </si>
   <si>
@@ -83,6 +80,9 @@
   </si>
   <si>
     <t>DayTona:60</t>
+  </si>
+  <si>
+    <t>Reverso:250</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="D1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +498,7 @@
     <row r="1" spans="4:15" x14ac:dyDescent="0.25">
       <c r="L1" t="str">
         <f>_xll.oxlDictionary(L3:N3,L4:N4)</f>
-        <v>Dictionary_Inventory_$0$11:1</v>
+        <v>Dictionary_Inventory_$0$11:2</v>
       </c>
     </row>
     <row r="3" spans="4:15" x14ac:dyDescent="0.25">
@@ -520,7 +520,7 @@
         <v>11</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N4" t="s">
         <v>12</v>
@@ -529,25 +529,25 @@
     <row r="5" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D5" t="str">
         <f>_xll.oxlArray(D14:F14)</f>
-        <v>Array_Inventory_$4$3:1</v>
+        <v>Array_Inventory_$4$3:2</v>
       </c>
     </row>
     <row r="7" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D7" t="str">
         <f>_xll.oxlArray(D10:E12)</f>
-        <v>Array_Inventory_$6$3:9</v>
+        <v>Array_Inventory_$6$3:4</v>
       </c>
       <c r="G7" t="str">
         <f>_xll.oxlDictionary(G10:H12)</f>
-        <v>Dictionary_Inventory_$6$6:1</v>
+        <v>Dictionary_Inventory_$6$6:2</v>
       </c>
       <c r="J7" t="str">
         <f>_xll.oxlDictionary($J$10:$J$12,K10:K12)</f>
-        <v>Dictionary_Inventory_$6$9:1</v>
+        <v>Dictionary_Inventory_$6$9:2</v>
       </c>
       <c r="K7" t="str">
         <f>_xll.oxlDictionary($J$10:$J$12,L10:L12)</f>
-        <v>Dictionary_Inventory_$6$10:1</v>
+        <v>Dictionary_Inventory_$6$10:2</v>
       </c>
       <c r="N7" t="str">
         <f t="array" ref="N7:O9">_xll.oxlDisplay(L1)</f>
@@ -593,7 +593,7 @@
         <v>11</v>
       </c>
       <c r="L10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="4:15" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
         <v>14</v>
       </c>
       <c r="L11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="4:15" x14ac:dyDescent="0.25">
@@ -639,7 +639,7 @@
         <v>12</v>
       </c>
       <c r="L12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="4:15" x14ac:dyDescent="0.25">
@@ -719,7 +719,7 @@
         <v>JLC</v>
       </c>
       <c r="K19" t="str">
-        <v>Reverso:9</v>
+        <v>Reverso:250</v>
       </c>
     </row>
     <row r="20" spans="10:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished initliazation of everythin needed for the project
</commit_message>
<xml_diff>
--- a/sheets/array_test_sheet.xlsx
+++ b/sheets/array_test_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ExcelPy\OdinAnalytics\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0281AAF1-F172-4AF7-9424-A0BA92057CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D773EC97-7C35-4240-B8F7-F5916D35DBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{CC038B3D-5DA1-43AC-BE17-600265123F86}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CC038B3D-5DA1-43AC-BE17-600265123F86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t xml:space="preserve">apple </t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Reverso:250</t>
+  </si>
+  <si>
+    <t>Polaris:90</t>
   </si>
 </sst>
 </file>
@@ -437,17 +440,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DFABD2-AE01-4866-8EEF-6EB1F781458C}">
   <dimension ref="B7:C9"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" t="str">
         <f t="array" ref="B7:C9">_xll.oxlDisplay(Inventory!D7)</f>
         <v>jack fruit</v>
@@ -456,7 +459,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" t="str">
         <v xml:space="preserve">apple </v>
       </c>
@@ -464,7 +467,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="str">
         <v>banna</v>
       </c>
@@ -481,27 +484,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C818C1D-2C17-41AA-9577-0406209DFD12}">
   <dimension ref="D1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:15" x14ac:dyDescent="0.3">
       <c r="L1" t="str">
         <f>_xll.oxlDictionary(L3:N3,L4:N4)</f>
-        <v>Dictionary_Inventory_$0$11:2</v>
-      </c>
-    </row>
-    <row r="3" spans="4:15" x14ac:dyDescent="0.25">
+        <v>Dictionary_Inventory_$0$11:0</v>
+      </c>
+    </row>
+    <row r="3" spans="4:15" x14ac:dyDescent="0.3">
       <c r="J3" s="1">
         <v>44999</v>
       </c>
@@ -515,7 +518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:15" x14ac:dyDescent="0.3">
       <c r="L4" t="s">
         <v>11</v>
       </c>
@@ -526,20 +529,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D5" t="str">
         <f>_xll.oxlArray(D14:F14)</f>
-        <v>Array_Inventory_$4$3:2</v>
-      </c>
-    </row>
-    <row r="7" spans="4:15" x14ac:dyDescent="0.25">
+        <v>Array_Inventory_$4$3:0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D7" t="str">
         <f>_xll.oxlArray(D10:E12)</f>
-        <v>Array_Inventory_$6$3:4</v>
+        <v>Array_Inventory_$6$3:0</v>
       </c>
       <c r="G7" t="str">
         <f>_xll.oxlDictionary(G10:H12)</f>
-        <v>Dictionary_Inventory_$6$6:2</v>
+        <v>Dictionary_Inventory_$6$6:0</v>
       </c>
       <c r="J7" t="str">
         <f>_xll.oxlDictionary($J$10:$J$12,K10:K12)</f>
@@ -547,7 +550,7 @@
       </c>
       <c r="K7" t="str">
         <f>_xll.oxlDictionary($J$10:$J$12,L10:L12)</f>
-        <v>Dictionary_Inventory_$6$10:2</v>
+        <v>Dictionary_Inventory_$6$10:0</v>
       </c>
       <c r="N7" t="str">
         <f t="array" ref="N7:O9">_xll.oxlDisplay(L1)</f>
@@ -557,7 +560,7 @@
         <v>Royal Oak: 50</v>
       </c>
     </row>
-    <row r="8" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:15" x14ac:dyDescent="0.3">
       <c r="N8" t="str">
         <v>JLC</v>
       </c>
@@ -565,7 +568,7 @@
         <v>Polaris:6</v>
       </c>
     </row>
-    <row r="9" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:15" x14ac:dyDescent="0.3">
       <c r="N9" t="str">
         <v>Rolex</v>
       </c>
@@ -573,7 +576,7 @@
         <v>DayTona:60</v>
       </c>
     </row>
-    <row r="10" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>2</v>
       </c>
@@ -590,13 +593,13 @@
         <v>8</v>
       </c>
       <c r="K10" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="L10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>0</v>
       </c>
@@ -619,7 +622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>1</v>
       </c>
@@ -642,7 +645,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D14" t="str">
         <f t="array" ref="D14:E16">_xll.oxlDisplay(D7)</f>
         <v>jack fruit</v>
@@ -665,7 +668,7 @@
         <v>Royal Oak: 50</v>
       </c>
     </row>
-    <row r="15" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D15" t="str">
         <v xml:space="preserve">apple </v>
       </c>
@@ -682,10 +685,10 @@
         <v>JLC</v>
       </c>
       <c r="K15" t="str">
-        <v>Polaris:6</v>
-      </c>
-    </row>
-    <row r="16" spans="4:15" x14ac:dyDescent="0.25">
+        <v>Polaris:90</v>
+      </c>
+    </row>
+    <row r="16" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D16" t="str">
         <v>banna</v>
       </c>
@@ -705,7 +708,7 @@
         <v>Submariner:15</v>
       </c>
     </row>
-    <row r="18" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:11" x14ac:dyDescent="0.3">
       <c r="J18" t="str">
         <f t="array" ref="J18:K20">_xll.oxlDisplay(K7)</f>
         <v>AP</v>
@@ -714,7 +717,7 @@
         <v>Royal Oak:20</v>
       </c>
     </row>
-    <row r="19" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="10:11" x14ac:dyDescent="0.3">
       <c r="J19" t="str">
         <v>JLC</v>
       </c>
@@ -722,7 +725,7 @@
         <v>Reverso:250</v>
       </c>
     </row>
-    <row r="20" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="10:11" x14ac:dyDescent="0.3">
       <c r="J20" t="str">
         <v>Rolex</v>
       </c>

</xml_diff>

<commit_message>
Fixed a bug withthe object creation counter
</commit_message>
<xml_diff>
--- a/sheets/array_test_sheet.xlsx
+++ b/sheets/array_test_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ExcelPy\OdinAnalytics\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D773EC97-7C35-4240-B8F7-F5916D35DBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B427C76-CCC7-4488-8456-1C85C045C34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CC038B3D-5DA1-43AC-BE17-600265123F86}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{CC038B3D-5DA1-43AC-BE17-600265123F86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t xml:space="preserve">apple </t>
   </si>
@@ -37,21 +37,6 @@
     <t>jack fruit</t>
   </si>
   <si>
-    <t>Curt</t>
-  </si>
-  <si>
-    <t>Ryan</t>
-  </si>
-  <si>
-    <t>Associate</t>
-  </si>
-  <si>
-    <t>Driector</t>
-  </si>
-  <si>
-    <t>Managing Director</t>
-  </si>
-  <si>
     <t>JLC</t>
   </si>
   <si>
@@ -65,9 +50,6 @@
   </si>
   <si>
     <t>Royal Oak: 50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mike </t>
   </si>
   <si>
     <t>Submariner:15</t>
@@ -440,26 +422,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DFABD2-AE01-4866-8EEF-6EB1F781458C}">
   <dimension ref="B7:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C9"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
         <f t="array" ref="B7:C9">_xll.oxlDisplay(Inventory!D7)</f>
         <v>jack fruit</v>
       </c>
       <c r="C7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
         <v xml:space="preserve">apple </v>
       </c>
@@ -467,7 +449,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
         <v>banna</v>
       </c>
@@ -482,124 +464,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C818C1D-2C17-41AA-9577-0406209DFD12}">
-  <dimension ref="D1:O20"/>
+  <dimension ref="D1:L20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="L1" t="str">
-        <f>_xll.oxlDictionary(L3:N3,L4:N4)</f>
-        <v>Dictionary_Inventory_$0$11:0</v>
-      </c>
-    </row>
-    <row r="3" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="J3" s="1">
+    <row r="1" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I1" t="str">
+        <f>_xll.oxlDictionary(I3:K3,I4:K4)</f>
+        <v>Dictionary_Inventory_$0$8:0</v>
+      </c>
+    </row>
+    <row r="3" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G3" s="1">
         <v>44999</v>
       </c>
-      <c r="L3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="L4" t="s">
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
         <v>11</v>
       </c>
-      <c r="M4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D5" t="str">
         <f>_xll.oxlArray(D14:F14)</f>
-        <v>Array_Inventory_$4$3:0</v>
-      </c>
-    </row>
-    <row r="7" spans="4:15" x14ac:dyDescent="0.3">
+        <v>Array_Inventory_$4$3:2</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D7" t="str">
         <f>_xll.oxlArray(D10:E12)</f>
-        <v>Array_Inventory_$6$3:0</v>
+        <v>Array_Inventory_$6$3:5</v>
       </c>
       <c r="G7" t="str">
-        <f>_xll.oxlDictionary(G10:H12)</f>
-        <v>Dictionary_Inventory_$6$6:0</v>
-      </c>
-      <c r="J7" t="str">
-        <f>_xll.oxlDictionary($J$10:$J$12,K10:K12)</f>
-        <v>Dictionary_Inventory_$6$9:2</v>
+        <f>_xll.oxlDictionary($G$10:$G$12,H10:H12)</f>
+        <v>Dictionary_Inventory_$6$6:1</v>
+      </c>
+      <c r="H7" t="str">
+        <f>_xll.oxlDictionary($G$10:$G$12,I10:I12)</f>
+        <v>Dictionary_Inventory_$6$7:0</v>
       </c>
       <c r="K7" t="str">
-        <f>_xll.oxlDictionary($J$10:$J$12,L10:L12)</f>
-        <v>Dictionary_Inventory_$6$10:0</v>
-      </c>
-      <c r="N7" t="str">
-        <f t="array" ref="N7:O9">_xll.oxlDisplay(L1)</f>
+        <f t="array" ref="K7:L9">_xll.oxlDisplay(I1)</f>
         <v>AP</v>
       </c>
-      <c r="O7" t="str">
+      <c r="L7" t="str">
         <v>Royal Oak: 50</v>
       </c>
     </row>
-    <row r="8" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="N8" t="str">
+    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="K8" t="str">
         <v>JLC</v>
       </c>
-      <c r="O8" t="str">
+      <c r="L8" t="str">
         <v>Polaris:6</v>
       </c>
     </row>
-    <row r="9" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="N9" t="str">
+    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="K9" t="str">
         <v>Rolex</v>
       </c>
-      <c r="O9" t="str">
+      <c r="L9" t="str">
         <v>DayTona:60</v>
       </c>
     </row>
-    <row r="10" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>2</v>
       </c>
       <c r="E10">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G10" t="s">
         <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="4:15" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>0</v>
       </c>
@@ -607,22 +579,16 @@
         <v>170</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
         <v>9</v>
       </c>
-      <c r="K11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="4:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>1</v>
       </c>
@@ -630,45 +596,32 @@
         <v>120</v>
       </c>
       <c r="G12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" t="s">
         <v>10</v>
       </c>
-      <c r="K12" t="s">
-        <v>12</v>
-      </c>
-      <c r="L12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="4:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D14" t="str">
         <f t="array" ref="D14:E16">_xll.oxlDisplay(D7)</f>
         <v>jack fruit</v>
       </c>
       <c r="E14">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G14" t="str">
-        <f t="array" ref="G14:H16">_xll.oxlDisplay((G7))</f>
-        <v>Curt</v>
+        <f t="array" ref="G14:H16">_xll.oxlDisplay(G7)</f>
+        <v>AP</v>
       </c>
       <c r="H14" t="str">
-        <v>Managing Director</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="array" ref="J14:K16">_xll.oxlDisplay(J7)</f>
-        <v>AP</v>
-      </c>
-      <c r="K14" t="str">
         <v>Royal Oak: 50</v>
       </c>
     </row>
-    <row r="15" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D15" t="str">
         <v xml:space="preserve">apple </v>
       </c>
@@ -676,19 +629,13 @@
         <v>170</v>
       </c>
       <c r="G15" t="str">
-        <v xml:space="preserve">Mike </v>
+        <v>JLC</v>
       </c>
       <c r="H15" t="str">
-        <v>Driector</v>
-      </c>
-      <c r="J15" t="str">
-        <v>JLC</v>
-      </c>
-      <c r="K15" t="str">
         <v>Polaris:90</v>
       </c>
     </row>
-    <row r="16" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D16" t="str">
         <v>banna</v>
       </c>
@@ -696,40 +643,34 @@
         <v>120</v>
       </c>
       <c r="G16" t="str">
-        <v>Ryan</v>
+        <v>Rolex</v>
       </c>
       <c r="H16" t="str">
-        <v>Associate</v>
-      </c>
-      <c r="J16" t="str">
+        <v>Submariner:15</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G18" t="str">
+        <f t="array" ref="G18:H20">_xll.oxlDisplay(H7)</f>
+        <v>AP</v>
+      </c>
+      <c r="H18" t="str">
+        <v>Royal Oak:20</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G19" t="str">
+        <v>JLC</v>
+      </c>
+      <c r="H19" t="str">
+        <v>Reverso:250</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G20" t="str">
         <v>Rolex</v>
       </c>
-      <c r="K16" t="str">
-        <v>Submariner:15</v>
-      </c>
-    </row>
-    <row r="18" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J18" t="str">
-        <f t="array" ref="J18:K20">_xll.oxlDisplay(K7)</f>
-        <v>AP</v>
-      </c>
-      <c r="K18" t="str">
-        <v>Royal Oak:20</v>
-      </c>
-    </row>
-    <row r="19" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J19" t="str">
-        <v>JLC</v>
-      </c>
-      <c r="K19" t="str">
-        <v>Reverso:250</v>
-      </c>
-    </row>
-    <row r="20" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J20" t="str">
-        <v>Rolex</v>
-      </c>
-      <c r="K20" t="str">
+      <c r="H20" t="str">
         <v>Oyster Perpetual:15</v>
       </c>
     </row>

</xml_diff>